<commit_message>
update data feeds and add vaccination trends
</commit_message>
<xml_diff>
--- a/newton.xlsx
+++ b/newton.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Documents/My R/covid19/covid19code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Documents/My R/covid19local/covid19code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890257DD-FFF0-D548-9E23-AFED1B4B26CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5422CC-70C9-8441-9CE8-4B946E33E6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="1380" windowWidth="35000" windowHeight="30280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31960" windowHeight="36000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="newton" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="newton" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -589,6 +590,917 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Newton</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Case Restatements - 5/28/2020</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>newton!$J$3:$J$83</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="81"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>newton!$K$3:$K$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF44-ED4C-A65B-E722EAD2F8AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="233307087"/>
+        <c:axId val="233308719"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="233307087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233308719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="233308719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233307087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{75F5B6EC-E65B-054A-B9A2-EE0BFC43086B}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="186" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8678333" cy="6295376"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B139E733-0FEF-F549-AA1C-B1BF0A21F3EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -886,15 +1798,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +1823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43889</v>
       </c>
@@ -929,8 +1841,9 @@
         <f>SUM($D$2:D2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43890</v>
       </c>
@@ -948,8 +1861,9 @@
         <f>SUM($D$2:D3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43891</v>
       </c>
@@ -967,8 +1881,9 @@
         <f>SUM($D$2:D4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43892</v>
       </c>
@@ -986,8 +1901,9 @@
         <f>SUM($D$2:D5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43893</v>
       </c>
@@ -1005,8 +1921,9 @@
         <f>SUM($D$2:D6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43894</v>
       </c>
@@ -1024,8 +1941,9 @@
         <f>SUM($D$2:D7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43895</v>
       </c>
@@ -1043,8 +1961,9 @@
         <f>SUM($D$2:D8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43896</v>
       </c>
@@ -1062,8 +1981,9 @@
         <f>SUM($D$2:D9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43897</v>
       </c>
@@ -1081,8 +2001,9 @@
         <f>SUM($D$2:D10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43898</v>
       </c>
@@ -1100,8 +2021,9 @@
         <f>SUM($D$2:D11)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43899</v>
       </c>
@@ -1119,8 +2041,9 @@
         <f>SUM($D$2:D12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43900</v>
       </c>
@@ -1138,8 +2061,9 @@
         <f>SUM($D$2:D13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43901</v>
       </c>
@@ -1157,8 +2081,9 @@
         <f>SUM($D$2:D14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43902</v>
       </c>
@@ -1176,8 +2101,9 @@
         <f>SUM($D$2:D15)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43903</v>
       </c>
@@ -1195,8 +2121,9 @@
         <f>SUM($D$2:D16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43904</v>
       </c>
@@ -1214,8 +2141,9 @@
         <f>SUM($D$2:D17)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43905</v>
       </c>
@@ -1233,8 +2161,9 @@
         <f>SUM($D$2:D18)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43906</v>
       </c>
@@ -1252,8 +2181,9 @@
         <f>SUM($D$2:D19)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43907</v>
       </c>
@@ -1271,8 +2201,9 @@
         <f>SUM($D$2:D20)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43908</v>
       </c>
@@ -1290,8 +2221,9 @@
         <f>SUM($D$2:D21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43909</v>
       </c>
@@ -1309,8 +2241,9 @@
         <f>SUM($D$2:D22)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43910</v>
       </c>
@@ -1328,8 +2261,9 @@
         <f>SUM($D$2:D23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43911</v>
       </c>
@@ -1347,8 +2281,9 @@
         <f>SUM($D$2:D24)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43912</v>
       </c>
@@ -1366,8 +2301,9 @@
         <f>SUM($D$2:D25)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43913</v>
       </c>
@@ -1385,8 +2321,9 @@
         <f>SUM($D$2:D26)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43914</v>
       </c>
@@ -1404,8 +2341,9 @@
         <f>SUM($D$2:D27)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43915</v>
       </c>
@@ -1423,8 +2361,9 @@
         <f>SUM($D$2:D28)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43916</v>
       </c>
@@ -1442,8 +2381,9 @@
         <f>SUM($D$2:D29)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43917</v>
       </c>
@@ -1461,17 +2401,18 @@
         <f>SUM($D$2:D30)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43918</v>
       </c>
       <c r="B31">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31">
         <f>SUM($B$2:B31)</f>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1480,8 +2421,9 @@
         <f>SUM($D$2:D31)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43919</v>
       </c>
@@ -1490,7 +2432,7 @@
       </c>
       <c r="C32">
         <f>SUM($B$2:B32)</f>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1499,8 +2441,9 @@
         <f>SUM($D$2:D32)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43920</v>
       </c>
@@ -1509,7 +2452,7 @@
       </c>
       <c r="C33">
         <f>SUM($B$2:B33)</f>
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1518,13 +2461,14 @@
         <f>SUM($D$2:D33)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43921</v>
       </c>
       <c r="B34">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34">
         <f>SUM($B$2:B34)</f>
@@ -1537,17 +2481,18 @@
         <f>SUM($D$2:D34)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43922</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <f>SUM($B$2:B35)</f>
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1556,17 +2501,18 @@
         <f>SUM($D$2:D35)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43923</v>
       </c>
       <c r="B36">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C36">
         <f>SUM($B$2:B36)</f>
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1575,17 +2521,18 @@
         <f>SUM($D$2:D36)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43924</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <f>SUM($B$2:B37)</f>
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1594,8 +2541,9 @@
         <f>SUM($D$2:D37)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43925</v>
       </c>
@@ -1604,7 +2552,7 @@
       </c>
       <c r="C38">
         <f>SUM($B$2:B38)</f>
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1613,8 +2561,9 @@
         <f>SUM($D$2:D38)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43926</v>
       </c>
@@ -1623,7 +2572,7 @@
       </c>
       <c r="C39">
         <f>SUM($B$2:B39)</f>
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1632,17 +2581,18 @@
         <f>SUM($D$2:D39)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43927</v>
       </c>
       <c r="B40">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40">
         <f>SUM($B$2:B40)</f>
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1651,17 +2601,18 @@
         <f>SUM($D$2:D40)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43928</v>
       </c>
       <c r="B41">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C41">
         <f>SUM($B$2:B41)</f>
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1670,8 +2621,9 @@
         <f>SUM($D$2:D41)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43929</v>
       </c>
@@ -1680,18 +2632,19 @@
       </c>
       <c r="C42">
         <f>SUM($B$2:B42)</f>
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="D42">
-        <f t="shared" ref="D40:D47" si="0">22/7</f>
+        <f t="shared" ref="D42:D47" si="0">22/7</f>
         <v>3.1428571428571428</v>
       </c>
       <c r="E42">
         <f>SUM($D$2:D42)</f>
         <v>6.1428571428571423</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43930</v>
       </c>
@@ -1700,7 +2653,7 @@
       </c>
       <c r="C43">
         <f>SUM($B$2:B43)</f>
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
@@ -1710,8 +2663,9 @@
         <f>SUM($D$2:D43)</f>
         <v>9.2857142857142847</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43931</v>
       </c>
@@ -1720,7 +2674,7 @@
       </c>
       <c r="C44">
         <f>SUM($B$2:B44)</f>
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
@@ -1730,8 +2684,9 @@
         <f>SUM($D$2:D44)</f>
         <v>12.428571428571427</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43932</v>
       </c>
@@ -1740,7 +2695,7 @@
       </c>
       <c r="C45">
         <f>SUM($B$2:B45)</f>
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
@@ -1750,8 +2705,9 @@
         <f>SUM($D$2:D45)</f>
         <v>15.571428571428569</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43933</v>
       </c>
@@ -1760,7 +2716,7 @@
       </c>
       <c r="C46">
         <f>SUM($B$2:B46)</f>
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
@@ -1770,8 +2726,9 @@
         <f>SUM($D$2:D46)</f>
         <v>18.714285714285712</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43934</v>
       </c>
@@ -1780,7 +2737,7 @@
       </c>
       <c r="C47">
         <f>SUM($B$2:B47)</f>
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
@@ -1790,8 +2747,9 @@
         <f>SUM($D$2:D47)</f>
         <v>21.857142857142854</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43935</v>
       </c>
@@ -1800,7 +2758,7 @@
       </c>
       <c r="C48">
         <f>SUM($B$2:B48)</f>
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="D48">
         <f>22/7</f>
@@ -1810,17 +2768,18 @@
         <f>SUM($D$2:D48)</f>
         <v>24.999999999999996</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43936</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49">
         <f>SUM($B$2:B49)</f>
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="D49">
         <f t="shared" ref="D49:D54" si="1">33/7</f>
@@ -1830,17 +2789,18 @@
         <f>SUM($D$2:D49)</f>
         <v>29.714285714285712</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43937</v>
       </c>
       <c r="B50">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C50">
         <f>SUM($B$2:B50)</f>
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
@@ -1850,17 +2810,18 @@
         <f>SUM($D$2:D50)</f>
         <v>34.428571428571423</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43938</v>
       </c>
       <c r="B51">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <f>SUM($B$2:B51)</f>
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
@@ -1870,17 +2831,18 @@
         <f>SUM($D$2:D51)</f>
         <v>39.142857142857139</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43939</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C52">
         <f>SUM($B$2:B52)</f>
-        <v>547</v>
+        <v>560</v>
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
@@ -1890,17 +2852,18 @@
         <f>SUM($D$2:D52)</f>
         <v>43.857142857142854</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43940</v>
       </c>
       <c r="B53">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C53">
         <f>SUM($B$2:B53)</f>
-        <v>558</v>
+        <v>572</v>
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
@@ -1910,8 +2873,9 @@
         <f>SUM($D$2:D53)</f>
         <v>48.571428571428569</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43941</v>
       </c>
@@ -1920,7 +2884,7 @@
       </c>
       <c r="C54">
         <f>SUM($B$2:B54)</f>
-        <v>569</v>
+        <v>583</v>
       </c>
       <c r="D54">
         <f t="shared" si="1"/>
@@ -1930,8 +2894,9 @@
         <f>SUM($D$2:D54)</f>
         <v>53.285714285714285</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43942</v>
       </c>
@@ -1940,7 +2905,7 @@
       </c>
       <c r="C55">
         <f>SUM($B$2:B55)</f>
-        <v>581</v>
+        <v>595</v>
       </c>
       <c r="D55">
         <f>33/7</f>
@@ -1950,8 +2915,9 @@
         <f>SUM($D$2:D55)</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43943</v>
       </c>
@@ -1960,7 +2926,7 @@
       </c>
       <c r="C56">
         <f>SUM($B$2:B56)</f>
-        <v>593</v>
+        <v>607</v>
       </c>
       <c r="D56">
         <f t="shared" ref="D56:D61" si="2">13/7</f>
@@ -1970,17 +2936,18 @@
         <f>SUM($D$2:D56)</f>
         <v>59.857142857142854</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43944</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C57">
         <f>SUM($B$2:B57)</f>
-        <v>599</v>
+        <v>614</v>
       </c>
       <c r="D57">
         <f t="shared" si="2"/>
@@ -1990,17 +2957,18 @@
         <f>SUM($D$2:D57)</f>
         <v>61.714285714285708</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43945</v>
       </c>
       <c r="B58">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C58">
         <f>SUM($B$2:B58)</f>
-        <v>603</v>
+        <v>620</v>
       </c>
       <c r="D58">
         <f t="shared" si="2"/>
@@ -2010,8 +2978,9 @@
         <f>SUM($D$2:D58)</f>
         <v>63.571428571428562</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43946</v>
       </c>
@@ -2020,7 +2989,7 @@
       </c>
       <c r="C59">
         <f>SUM($B$2:B59)</f>
-        <v>604</v>
+        <v>621</v>
       </c>
       <c r="D59">
         <f t="shared" si="2"/>
@@ -2030,17 +2999,18 @@
         <f>SUM($D$2:D59)</f>
         <v>65.428571428571416</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43947</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C60">
         <f>SUM($B$2:B60)</f>
-        <v>606</v>
+        <v>627</v>
       </c>
       <c r="D60">
         <f t="shared" si="2"/>
@@ -2050,17 +3020,18 @@
         <f>SUM($D$2:D60)</f>
         <v>67.285714285714278</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43948</v>
       </c>
       <c r="B61">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61">
         <f>SUM($B$2:B61)</f>
-        <v>620</v>
+        <v>642</v>
       </c>
       <c r="D61">
         <f t="shared" si="2"/>
@@ -2070,17 +3041,18 @@
         <f>SUM($D$2:D61)</f>
         <v>69.142857142857139</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43949</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C62">
         <f>SUM($B$2:B62)</f>
-        <v>623</v>
+        <v>647</v>
       </c>
       <c r="D62">
         <f>13/7</f>
@@ -2090,17 +3062,18 @@
         <f>SUM($D$2:D62)</f>
         <v>71</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43950</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C63">
         <f>SUM($B$2:B63)</f>
-        <v>631</v>
+        <v>654</v>
       </c>
       <c r="D63">
         <f t="shared" ref="D63:D68" si="3">15/7</f>
@@ -2110,17 +3083,18 @@
         <f>SUM($D$2:D63)</f>
         <v>73.142857142857139</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43951</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <f>SUM($B$2:B64)</f>
-        <v>636</v>
+        <v>657</v>
       </c>
       <c r="D64">
         <f t="shared" si="3"/>
@@ -2130,8 +3104,9 @@
         <f>SUM($D$2:D64)</f>
         <v>75.285714285714278</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43952</v>
       </c>
@@ -2140,7 +3115,7 @@
       </c>
       <c r="C65">
         <f>SUM($B$2:B65)</f>
-        <v>646</v>
+        <v>667</v>
       </c>
       <c r="D65">
         <f t="shared" si="3"/>
@@ -2150,17 +3125,18 @@
         <f>SUM($D$2:D65)</f>
         <v>77.428571428571416</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43953</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <f>SUM($B$2:B66)</f>
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="D66">
         <f t="shared" si="3"/>
@@ -2170,17 +3146,18 @@
         <f>SUM($D$2:D66)</f>
         <v>79.571428571428555</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43954</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C67">
         <f>SUM($B$2:B67)</f>
-        <v>652</v>
+        <v>676</v>
       </c>
       <c r="D67">
         <f t="shared" si="3"/>
@@ -2190,17 +3167,18 @@
         <f>SUM($D$2:D67)</f>
         <v>81.714285714285694</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43955</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C68">
         <f>SUM($B$2:B68)</f>
-        <v>658</v>
+        <v>679</v>
       </c>
       <c r="D68">
         <f t="shared" si="3"/>
@@ -2210,17 +3188,18 @@
         <f>SUM($D$2:D68)</f>
         <v>83.857142857142833</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43956</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69">
         <f>SUM($B$2:B69)</f>
-        <v>661</v>
+        <v>681</v>
       </c>
       <c r="D69">
         <f>15/7</f>
@@ -2230,17 +3209,18 @@
         <f>SUM($D$2:D69)</f>
         <v>85.999999999999972</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43957</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C70">
         <f>SUM($B$2:B70)</f>
-        <v>668</v>
+        <v>689</v>
       </c>
       <c r="D70">
         <f t="shared" ref="D70:D75" si="4">10/7</f>
@@ -2250,17 +3230,18 @@
         <f>SUM($D$2:D70)</f>
         <v>87.428571428571402</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43958</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C71">
         <f>SUM($B$2:B71)</f>
-        <v>674</v>
+        <v>692</v>
       </c>
       <c r="D71">
         <f t="shared" si="4"/>
@@ -2270,17 +3251,18 @@
         <f>SUM($D$2:D71)</f>
         <v>88.857142857142833</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43959</v>
       </c>
       <c r="B72">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C72">
         <f>SUM($B$2:B72)</f>
-        <v>682</v>
+        <v>695</v>
       </c>
       <c r="D72">
         <f t="shared" si="4"/>
@@ -2290,17 +3272,18 @@
         <f>SUM($D$2:D72)</f>
         <v>90.285714285714263</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43960</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C73">
         <f>SUM($B$2:B73)</f>
-        <v>682</v>
+        <v>697</v>
       </c>
       <c r="D73">
         <f t="shared" si="4"/>
@@ -2310,17 +3293,18 @@
         <f>SUM($D$2:D73)</f>
         <v>91.714285714285694</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43961</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C74">
         <f>SUM($B$2:B74)</f>
-        <v>684</v>
+        <v>698</v>
       </c>
       <c r="D74">
         <f t="shared" si="4"/>
@@ -2330,17 +3314,18 @@
         <f>SUM($D$2:D74)</f>
         <v>93.142857142857125</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43962</v>
       </c>
       <c r="B75">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C75">
         <f>SUM($B$2:B75)</f>
-        <v>690</v>
+        <v>702</v>
       </c>
       <c r="D75">
         <f t="shared" si="4"/>
@@ -2350,17 +3335,18 @@
         <f>SUM($D$2:D75)</f>
         <v>94.571428571428555</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43963</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C76">
         <f>SUM($B$2:B76)</f>
-        <v>690</v>
+        <v>704</v>
       </c>
       <c r="D76">
         <f>10/7</f>
@@ -2370,28 +3356,30 @@
         <f>SUM($D$2:D76)</f>
         <v>95.999999999999986</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43964</v>
       </c>
       <c r="B77">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77">
         <f>SUM($B$2:B77)</f>
-        <v>697</v>
+        <v>710</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D83" si="5">9/7</f>
+        <f t="shared" ref="D77:D82" si="5">9/7</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="E77">
         <f>SUM($D$2:D77)</f>
         <v>97.285714285714278</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43965</v>
       </c>
@@ -2400,7 +3388,7 @@
       </c>
       <c r="C78">
         <f>SUM($B$2:B78)</f>
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="D78">
         <f t="shared" si="5"/>
@@ -2410,17 +3398,18 @@
         <f>SUM($D$2:D78)</f>
         <v>98.571428571428569</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43966</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C79">
         <f>SUM($B$2:B79)</f>
-        <v>701</v>
+        <v>716</v>
       </c>
       <c r="D79">
         <f t="shared" si="5"/>
@@ -2430,17 +3419,18 @@
         <f>SUM($D$2:D79)</f>
         <v>99.857142857142861</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43967</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C80">
         <f>SUM($B$2:B80)</f>
-        <v>702</v>
+        <v>718</v>
       </c>
       <c r="D80">
         <f t="shared" si="5"/>
@@ -2450,8 +3440,9 @@
         <f>SUM($D$2:D80)</f>
         <v>101.14285714285715</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43968</v>
       </c>
@@ -2460,7 +3451,7 @@
       </c>
       <c r="C81">
         <f>SUM($B$2:B81)</f>
-        <v>703</v>
+        <v>719</v>
       </c>
       <c r="D81">
         <f t="shared" si="5"/>
@@ -2470,8 +3461,9 @@
         <f>SUM($D$2:D81)</f>
         <v>102.42857142857144</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43969</v>
       </c>
@@ -2480,7 +3472,7 @@
       </c>
       <c r="C82">
         <f>SUM($B$2:B82)</f>
-        <v>709</v>
+        <v>725</v>
       </c>
       <c r="D82">
         <f t="shared" si="5"/>
@@ -2490,17 +3482,18 @@
         <f>SUM($D$2:D82)</f>
         <v>103.71428571428574</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43970</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C83">
         <f>SUM($B$2:B83)</f>
-        <v>710</v>
+        <v>731</v>
       </c>
       <c r="D83">
         <f>9/7</f>
@@ -2510,252 +3503,286 @@
         <f>SUM($D$2:D83)</f>
         <v>105.00000000000003</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43971</v>
       </c>
-      <c r="B84" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C84" t="e">
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84">
         <f>SUM($B$2:B84)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D84" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E84" t="e">
+        <v>733</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ref="D84:D89" si="6">2/7</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E84">
         <f>SUM($D$2:D84)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105.28571428571432</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43972</v>
       </c>
-      <c r="B85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C85" t="e">
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85">
         <f>SUM($B$2:B85)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E85" t="e">
+        <v>736</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="6"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E85">
         <f>SUM($D$2:D85)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105.57142857142861</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43973</v>
       </c>
-      <c r="B86" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C86" t="e">
+      <c r="B86">
+        <v>9</v>
+      </c>
+      <c r="C86">
         <f>SUM($B$2:B86)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D86" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E86" t="e">
+        <v>745</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="6"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E86">
         <f>SUM($D$2:D86)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105.8571428571429</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43974</v>
       </c>
-      <c r="B87" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C87" t="e">
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
         <f>SUM($B$2:B87)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D87" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E87" t="e">
+        <v>747</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="6"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E87">
         <f>SUM($D$2:D87)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106.1428571428572</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43975</v>
       </c>
-      <c r="B88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C88" t="e">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
         <f>SUM($B$2:B88)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E88" t="e">
+        <v>748</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="6"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E88">
         <f>SUM($D$2:D88)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106.42857142857149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43976</v>
       </c>
-      <c r="B89" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C89" t="e">
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
         <f>SUM($B$2:B89)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D89" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E89" t="e">
+        <v>748</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="6"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E89">
         <f>SUM($D$2:D89)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106.71428571428578</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>43977</v>
       </c>
-      <c r="B90" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C90" t="e">
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="C90">
         <f>SUM($B$2:B90)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D90" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E90" t="e">
+        <v>752</v>
+      </c>
+      <c r="D90">
+        <f>2/7</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E90">
         <f>SUM($D$2:D90)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107.00000000000007</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43978</v>
       </c>
-      <c r="B91" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C91" t="e">
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91">
         <f>SUM($B$2:B91)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D91" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E91" t="e">
+        <v>754</v>
+      </c>
+      <c r="D91">
+        <f>9/7</f>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E91">
         <f>SUM($D$2:D91)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108.28571428571436</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>43979</v>
       </c>
-      <c r="B92" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C92" t="e">
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
         <f>SUM($B$2:B92)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D92" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E92" t="e">
+        <v>755</v>
+      </c>
+      <c r="D92">
+        <f t="shared" ref="D92:D97" si="7">9/7</f>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E92">
         <f>SUM($D$2:D92)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>109.57142857142865</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43980</v>
       </c>
-      <c r="B93" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C93" t="e">
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93">
         <f>SUM($B$2:B93)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D93" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E93" t="e">
+        <v>757</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="7"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E93">
         <f>SUM($D$2:D93)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>110.85714285714295</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43981</v>
       </c>
-      <c r="B94" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C94" t="e">
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
         <f>SUM($B$2:B94)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D94" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E94" t="e">
+        <v>757</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="7"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E94">
         <f>SUM($D$2:D94)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+        <v>112.14285714285724</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>43982</v>
       </c>
-      <c r="B95" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C95" t="e">
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
         <f>SUM($B$2:B95)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D95" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E95" t="e">
+        <v>758</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="7"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E95">
         <f>SUM($D$2:D95)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+        <v>113.42857142857153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>43983</v>
       </c>
-      <c r="B96" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C96" t="e">
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
         <f>SUM($B$2:B96)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D96" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E96" t="e">
+        <v>759</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="7"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E96">
         <f>SUM($D$2:D96)</f>
-        <v>#N/A</v>
+        <v>114.71428571428582</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <f>SUM($B$2:B97)</f>
+        <v>759</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="7"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="E97">
+        <f>SUM($D$2:D97)</f>
+        <v>116.00000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>